<commit_message>
Modificati i file excel e iniziato il testing
</commit_message>
<xml_diff>
--- a/data/modelli/modello1.xlsx
+++ b/data/modelli/modello1.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Modello</t>
   </si>
   <si>
-    <t>Servizi del municipio</t>
+    <t xml:space="preserve">Servizi del municipio</t>
   </si>
   <si>
-    <t>Come valuti il servizio di accoglienza</t>
+    <t xml:space="preserve">Come valuti il servizio di accoglienza</t>
   </si>
   <si>
     <t>Pessimo</t>
@@ -28,7 +30,7 @@
     <t>Negativo</t>
   </si>
   <si>
-    <t>Cosi cosi</t>
+    <t xml:space="preserve">Cosi cosi</t>
   </si>
   <si>
     <t>Buono</t>
@@ -37,28 +39,28 @@
     <t>Eccezionale</t>
   </si>
   <si>
-    <t>Come valuti l’ufficio tecnico</t>
+    <t xml:space="preserve">Come valuti l’ufficio tecnico</t>
   </si>
   <si>
-    <t>Come valuti l’ufficio anagrafe</t>
+    <t xml:space="preserve">Come valuti l’ufficio anagrafe</t>
   </si>
   <si>
-    <t>Come valuti l’ufficio tributi</t>
+    <t xml:space="preserve">Come valuti l’ufficio tributi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <color indexed="64"/>
+      <sz val="10.000000"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,34 +68,324 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="3">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -150,7 +442,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -176,7 +468,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -228,16 +520,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -253,7 +557,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -283,18 +587,22 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="38.57"/>
     <col customWidth="1" min="2" max="2" width="17.43"/>
@@ -306,9 +614,9 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1388,13 +1696,12 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0249999999999997" footer="0.0" header="0.0" left="0.7875000000000001" right="0.7875000000000001" top="1.0249999999999997"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.0249999999999997" bottom="1.0249999999999997" header="0" footer="0"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>